<commit_message>
New data generation method
</commit_message>
<xml_diff>
--- a/assets/cars.xlsx
+++ b/assets/cars.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aexra\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aexra\source\repos\etl\airflow-docker-test\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0036352C-967C-4305-9206-E55A902FF958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D1ECB4-A7C0-4DEF-988A-0265A5FF04DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{878BA8A0-CF4D-4C2F-BAC1-7E31EE170372}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>engine_volume</t>
   </si>
   <si>
-    <t>published_at</t>
-  </si>
-  <si>
     <t>Toyota</t>
   </si>
   <si>
@@ -201,6 +198,9 @@
   </si>
   <si>
     <t>1.3</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -577,12 +577,12 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="11.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -599,7 +599,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -607,13 +607,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2">
         <v>2022</v>
@@ -624,13 +624,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3">
         <v>2023</v>
@@ -641,13 +641,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E4">
         <v>2021</v>
@@ -658,13 +658,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="E5">
         <v>2023</v>
@@ -675,13 +675,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6">
         <v>2022</v>
@@ -692,13 +692,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7">
         <v>2021</v>
@@ -709,13 +709,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8">
         <v>2023</v>
@@ -726,13 +726,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9">
         <v>2022</v>
@@ -743,13 +743,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10">
         <v>2023</v>
@@ -760,13 +760,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11">
         <v>2021</v>
@@ -777,13 +777,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12">
         <v>2022</v>
@@ -794,13 +794,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
         <v>29</v>
       </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13">
         <v>2023</v>
@@ -811,13 +811,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
-        <v>32</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E14">
         <v>2021</v>
@@ -828,13 +828,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
         <v>33</v>
       </c>
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15">
         <v>2022</v>
@@ -845,13 +845,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
         <v>35</v>
       </c>
-      <c r="C16" t="s">
-        <v>36</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E16">
         <v>2023</v>
@@ -862,13 +862,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
         <v>37</v>
       </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E17">
         <v>2021</v>
@@ -879,13 +879,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18">
         <v>3008</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E18">
         <v>2022</v>
@@ -896,13 +896,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
         <v>40</v>
       </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
       <c r="D19" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19">
         <v>2021</v>
@@ -913,13 +913,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
         <v>42</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="E20">
         <v>2023</v>
@@ -930,13 +930,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
         <v>45</v>
       </c>
-      <c r="C21" t="s">
-        <v>46</v>
-      </c>
       <c r="D21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E21">
         <v>2022</v>

</xml_diff>